<commit_message>
added section on S&P500 pct drops
</commit_message>
<xml_diff>
--- a/my_exported_file.xlsx
+++ b/my_exported_file.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H315"/>
+  <dimension ref="A1:H316"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -487,7 +487,7 @@
         <v>20901500</v>
       </c>
       <c r="H4">
-        <v>364.4781494140625</v>
+        <v>364.4781799316406</v>
       </c>
     </row>
     <row r="5">
@@ -739,7 +739,7 @@
         <v>23392100</v>
       </c>
       <c r="H13">
-        <v>390.1641845703125</v>
+        <v>390.1642150878906</v>
       </c>
     </row>
     <row r="14">
@@ -795,7 +795,7 @@
         <v>27016900</v>
       </c>
       <c r="H15">
-        <v>392.7794189453125</v>
+        <v>392.7793884277344</v>
       </c>
     </row>
     <row r="16">
@@ -851,7 +851,7 @@
         <v>24867000</v>
       </c>
       <c r="H17">
-        <v>398.7724914550781</v>
+        <v>398.7724609375</v>
       </c>
     </row>
     <row r="18">
@@ -907,7 +907,7 @@
         <v>17803300</v>
       </c>
       <c r="H19">
-        <v>400.1295166015625</v>
+        <v>400.1295776367188</v>
       </c>
     </row>
     <row r="20">
@@ -991,7 +991,7 @@
         <v>47871100</v>
       </c>
       <c r="H22">
-        <v>393.8392944335938</v>
+        <v>393.8393249511719</v>
       </c>
     </row>
     <row r="23">
@@ -1019,7 +1019,7 @@
         <v>30657700</v>
       </c>
       <c r="H23">
-        <v>399.98095703125</v>
+        <v>399.9809875488281</v>
       </c>
     </row>
     <row r="24">
@@ -1047,7 +1047,7 @@
         <v>28245000</v>
       </c>
       <c r="H24">
-        <v>407.3509826660156</v>
+        <v>407.3509521484375</v>
       </c>
     </row>
     <row r="25">
@@ -1075,7 +1075,7 @@
         <v>25352300</v>
       </c>
       <c r="H25">
-        <v>401.8333740234375</v>
+        <v>401.8333435058594</v>
       </c>
     </row>
     <row r="26">
@@ -1131,7 +1131,7 @@
         <v>22340500</v>
       </c>
       <c r="H27">
-        <v>410.1543579101562</v>
+        <v>410.1543273925781</v>
       </c>
     </row>
     <row r="28">
@@ -1159,7 +1159,7 @@
         <v>21225300</v>
       </c>
       <c r="H28">
-        <v>410.2137451171875</v>
+        <v>410.2137756347656</v>
       </c>
     </row>
     <row r="29">
@@ -9196,6 +9196,34 @@
       </c>
       <c r="H315">
         <v>382.1400146484375</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B316" s="2">
+        <v>45750</v>
+      </c>
+      <c r="C316">
+        <v>374.7900085449219</v>
+      </c>
+      <c r="D316">
+        <v>377.4800109863281</v>
+      </c>
+      <c r="E316">
+        <v>369.3500061035156</v>
+      </c>
+      <c r="F316">
+        <v>373.1099853515625</v>
+      </c>
+      <c r="G316">
+        <v>30147000</v>
+      </c>
+      <c r="H316">
+        <v>373.1099853515625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final tweaks for session
</commit_message>
<xml_diff>
--- a/my_exported_file.xlsx
+++ b/my_exported_file.xlsx
@@ -487,7 +487,7 @@
         <v>20901500</v>
       </c>
       <c r="H4">
-        <v>364.4781799316406</v>
+        <v>364.4781494140625</v>
       </c>
     </row>
     <row r="5">
@@ -627,7 +627,7 @@
         <v>27850800</v>
       </c>
       <c r="H9">
-        <v>381.0111694335938</v>
+        <v>381.0111389160156</v>
       </c>
     </row>
     <row r="10">
@@ -655,7 +655,7 @@
         <v>21645700</v>
       </c>
       <c r="H10">
-        <v>384.8150329589844</v>
+        <v>384.8150024414062</v>
       </c>
     </row>
     <row r="11">
@@ -767,7 +767,7 @@
         <v>29272000</v>
       </c>
       <c r="H14">
-        <v>394.9190368652344</v>
+        <v>394.9190673828125</v>
       </c>
     </row>
     <row r="15">
@@ -823,7 +823,7 @@
         <v>20525900</v>
       </c>
       <c r="H16">
-        <v>395.1468811035156</v>
+        <v>395.1468505859375</v>
       </c>
     </row>
     <row r="17">
@@ -851,7 +851,7 @@
         <v>24867000</v>
       </c>
       <c r="H17">
-        <v>398.7724609375</v>
+        <v>398.7724304199219</v>
       </c>
     </row>
     <row r="18">
@@ -879,7 +879,7 @@
         <v>21021200</v>
       </c>
       <c r="H18">
-        <v>401.0606994628906</v>
+        <v>401.0607299804688</v>
       </c>
     </row>
     <row r="19">
@@ -935,7 +935,7 @@
         <v>24510200</v>
       </c>
       <c r="H20">
-        <v>405.8650512695312</v>
+        <v>405.8650817871094</v>
       </c>
     </row>
     <row r="21">
@@ -991,7 +991,7 @@
         <v>47871100</v>
       </c>
       <c r="H22">
-        <v>393.8393249511719</v>
+        <v>393.8392944335938</v>
       </c>
     </row>
     <row r="23">
@@ -1019,7 +1019,7 @@
         <v>30657700</v>
       </c>
       <c r="H23">
-        <v>399.9809875488281</v>
+        <v>399.9810180664062</v>
       </c>
     </row>
     <row r="24">
@@ -1047,7 +1047,7 @@
         <v>28245000</v>
       </c>
       <c r="H24">
-        <v>407.3509521484375</v>
+        <v>407.3509826660156</v>
       </c>
     </row>
     <row r="25">
@@ -1075,7 +1075,7 @@
         <v>25352300</v>
       </c>
       <c r="H25">
-        <v>401.8333435058594</v>
+        <v>401.8334045410156</v>
       </c>
     </row>
     <row r="26">
@@ -1103,7 +1103,7 @@
         <v>18382600</v>
       </c>
       <c r="H26">
-        <v>401.6748657226562</v>
+        <v>401.6748352050781</v>
       </c>
     </row>
     <row r="27">
@@ -1159,7 +1159,7 @@
         <v>21225300</v>
       </c>
       <c r="H28">
-        <v>410.2137756347656</v>
+        <v>410.2137451171875</v>
       </c>
     </row>
     <row r="29">
@@ -1215,7 +1215,7 @@
         <v>21202900</v>
       </c>
       <c r="H30">
-        <v>411.3529357910156</v>
+        <v>411.3529968261719</v>
       </c>
     </row>
     <row r="31">
@@ -1355,7 +1355,7 @@
         <v>24307900</v>
       </c>
       <c r="H35">
-        <v>399.7381286621094</v>
+        <v>399.7381591796875</v>
       </c>
     </row>
     <row r="36">
@@ -1383,7 +1383,7 @@
         <v>18631100</v>
       </c>
       <c r="H36">
-        <v>399.1327514648438</v>
+        <v>399.1327209472656</v>
       </c>
     </row>
     <row r="37">
@@ -1411,7 +1411,7 @@
         <v>27009900</v>
       </c>
       <c r="H37">
-        <v>408.5309753417969</v>
+        <v>408.531005859375</v>
       </c>
     </row>
     <row r="38">
@@ -1439,7 +1439,7 @@
         <v>16295900</v>
       </c>
       <c r="H38">
-        <v>407.23095703125</v>
+        <v>407.2308959960938</v>
       </c>
     </row>
     <row r="39">
@@ -1467,7 +1467,7 @@
         <v>16193500</v>
       </c>
       <c r="H39">
-        <v>404.4521789550781</v>
+        <v>404.4521484375</v>
       </c>
     </row>
     <row r="40">
@@ -1495,7 +1495,7 @@
         <v>14835800</v>
       </c>
       <c r="H40">
-        <v>404.3926086425781</v>
+        <v>404.3926391601562</v>
       </c>
     </row>
     <row r="41">
@@ -1523,7 +1523,7 @@
         <v>13183100</v>
       </c>
       <c r="H41">
-        <v>404.6307678222656</v>
+        <v>404.6307983398438</v>
       </c>
     </row>
     <row r="42">
@@ -1607,7 +1607,7 @@
         <v>17596000</v>
       </c>
       <c r="H44">
-        <v>411.7762756347656</v>
+        <v>411.7762451171875</v>
       </c>
     </row>
     <row r="45">
@@ -1635,7 +1635,7 @@
         <v>26919200</v>
       </c>
       <c r="H45">
-        <v>399.5991516113281</v>
+        <v>399.5992126464844</v>
       </c>
     </row>
     <row r="46">
@@ -1691,7 +1691,7 @@
         <v>18718500</v>
       </c>
       <c r="H47">
-        <v>406.0400695800781</v>
+        <v>406.0400390625</v>
       </c>
     </row>
     <row r="48">
@@ -1971,7 +1971,7 @@
         <v>21296200</v>
       </c>
       <c r="H57">
-        <v>426.1167297363281</v>
+        <v>426.1167602539062</v>
       </c>
     </row>
     <row r="58">
@@ -1999,7 +1999,7 @@
         <v>17636500</v>
       </c>
       <c r="H58">
-        <v>425.4915161132812</v>
+        <v>425.4915466308594</v>
       </c>
     </row>
     <row r="59">
@@ -2083,7 +2083,7 @@
         <v>16705000</v>
       </c>
       <c r="H61">
-        <v>418.2368774414062</v>
+        <v>418.2369079589844</v>
       </c>
     </row>
     <row r="62">
@@ -2251,7 +2251,7 @@
         <v>16544300</v>
       </c>
       <c r="H67">
-        <v>422.2959289550781</v>
+        <v>422.2958984375</v>
       </c>
     </row>
     <row r="68">
@@ -2307,7 +2307,7 @@
         <v>12512300</v>
       </c>
       <c r="H69">
-        <v>423.0501403808594</v>
+        <v>423.0501708984375</v>
       </c>
     </row>
     <row r="70">
@@ -2335,7 +2335,7 @@
         <v>16216600</v>
       </c>
       <c r="H70">
-        <v>420.0530700683594</v>
+        <v>420.0530395507812</v>
       </c>
     </row>
     <row r="71">
@@ -2363,7 +2363,7 @@
         <v>17966400</v>
       </c>
       <c r="H71">
-        <v>424.6876831054688</v>
+        <v>424.6876220703125</v>
       </c>
     </row>
     <row r="72">
@@ -2615,7 +2615,7 @@
         <v>15065300</v>
       </c>
       <c r="H80">
-        <v>405.9606018066406</v>
+        <v>405.9606628417969</v>
       </c>
     </row>
     <row r="81">
@@ -2643,7 +2643,7 @@
         <v>40586500</v>
       </c>
       <c r="H81">
-        <v>396.0165405273438</v>
+        <v>396.0165710449219</v>
       </c>
     </row>
     <row r="82">
@@ -2699,7 +2699,7 @@
         <v>19582100</v>
       </c>
       <c r="H83">
-        <v>399.2022094726562</v>
+        <v>399.2022399902344</v>
       </c>
     </row>
     <row r="84">
@@ -2727,7 +2727,7 @@
         <v>28781400</v>
       </c>
       <c r="H84">
-        <v>386.3800964355469</v>
+        <v>386.380126953125</v>
       </c>
     </row>
     <row r="85">
@@ -2755,7 +2755,7 @@
         <v>23562500</v>
       </c>
       <c r="H85">
-        <v>391.9476013183594</v>
+        <v>391.9476318359375</v>
       </c>
     </row>
     <row r="86">
@@ -2783,7 +2783,7 @@
         <v>17709400</v>
       </c>
       <c r="H86">
-        <v>394.8256530761719</v>
+        <v>394.8255920410156</v>
       </c>
     </row>
     <row r="87">
@@ -2867,7 +2867,7 @@
         <v>20018200</v>
       </c>
       <c r="H89">
-        <v>406.238525390625</v>
+        <v>406.2384948730469</v>
       </c>
     </row>
     <row r="90">
@@ -2923,7 +2923,7 @@
         <v>14689700</v>
       </c>
       <c r="H91">
-        <v>409.1959228515625</v>
+        <v>409.1959533691406</v>
       </c>
     </row>
     <row r="92">
@@ -3035,7 +3035,7 @@
         <v>22239500</v>
       </c>
       <c r="H95">
-        <v>420.6317443847656</v>
+        <v>420.6317138671875</v>
       </c>
     </row>
     <row r="96">
@@ -3147,7 +3147,7 @@
         <v>21453300</v>
       </c>
       <c r="H99">
-        <v>426.5572509765625</v>
+        <v>426.5572814941406</v>
       </c>
     </row>
     <row r="100">
@@ -3175,7 +3175,7 @@
         <v>18073700</v>
       </c>
       <c r="H100">
-        <v>428.0287170410156</v>
+        <v>428.0286865234375</v>
       </c>
     </row>
     <row r="101">
@@ -3259,7 +3259,7 @@
         <v>15718000</v>
       </c>
       <c r="H103">
-        <v>427.8298645019531</v>
+        <v>427.829833984375</v>
       </c>
     </row>
     <row r="104">
@@ -3707,7 +3707,7 @@
         <v>19877400</v>
       </c>
       <c r="H119">
-        <v>443.1208801269531</v>
+        <v>443.120849609375</v>
       </c>
     </row>
     <row r="120">
@@ -3763,7 +3763,7 @@
         <v>15913700</v>
       </c>
       <c r="H121">
-        <v>445.0794677734375</v>
+        <v>445.0794982910156</v>
       </c>
     </row>
     <row r="122">
@@ -3875,7 +3875,7 @@
         <v>28362300</v>
       </c>
       <c r="H125">
-        <v>444.3636169433594</v>
+        <v>444.3636474609375</v>
       </c>
     </row>
     <row r="126">
@@ -3903,7 +3903,7 @@
         <v>17662800</v>
       </c>
       <c r="H126">
-        <v>454.0870056152344</v>
+        <v>454.0870361328125</v>
       </c>
     </row>
     <row r="127">
@@ -4099,7 +4099,7 @@
         <v>23111200</v>
       </c>
       <c r="H133">
-        <v>452.0687866210938</v>
+        <v>452.0687561035156</v>
       </c>
     </row>
     <row r="134">
@@ -4155,7 +4155,7 @@
         <v>14429400</v>
       </c>
       <c r="H135">
-        <v>451.3330383300781</v>
+        <v>451.3330688476562</v>
       </c>
     </row>
     <row r="136">
@@ -4435,7 +4435,7 @@
         <v>15125800</v>
       </c>
       <c r="H145">
-        <v>424.2606506347656</v>
+        <v>424.2606201171875</v>
       </c>
     </row>
     <row r="146">
@@ -4491,7 +4491,7 @@
         <v>42891400</v>
       </c>
       <c r="H147">
-        <v>415.9291076660156</v>
+        <v>415.9291381835938</v>
       </c>
     </row>
     <row r="148">
@@ -4519,7 +4519,7 @@
         <v>30296400</v>
       </c>
       <c r="H148">
-        <v>414.6962585449219</v>
+        <v>414.6962890625</v>
       </c>
     </row>
     <row r="149">
@@ -4575,7 +4575,7 @@
         <v>40709200</v>
       </c>
       <c r="H150">
-        <v>392.8633728027344</v>
+        <v>392.8633422851562</v>
       </c>
     </row>
     <row r="151">
@@ -4659,7 +4659,7 @@
         <v>20203000</v>
       </c>
       <c r="H153">
-        <v>400.3597106933594</v>
+        <v>400.3597412109375</v>
       </c>
     </row>
     <row r="154">
@@ -4855,7 +4855,7 @@
         <v>15234000</v>
       </c>
       <c r="H160">
-        <v>419.8460693359375</v>
+        <v>419.8460998535156</v>
       </c>
     </row>
     <row r="161">
@@ -4939,7 +4939,7 @@
         <v>19361900</v>
       </c>
       <c r="H163">
-        <v>413.8899536132812</v>
+        <v>413.8899841308594</v>
       </c>
     </row>
     <row r="164">
@@ -4995,7 +4995,7 @@
         <v>13152800</v>
       </c>
       <c r="H165">
-        <v>411.8382263183594</v>
+        <v>411.8381958007812</v>
       </c>
     </row>
     <row r="166">
@@ -5023,7 +5023,7 @@
         <v>13492900</v>
       </c>
       <c r="H166">
-        <v>412.1868286132812</v>
+        <v>412.1867980957031</v>
       </c>
     </row>
     <row r="167">
@@ -5051,7 +5051,7 @@
         <v>14882700</v>
       </c>
       <c r="H167">
-        <v>408.9597473144531</v>
+        <v>408.9597778320312</v>
       </c>
     </row>
     <row r="168">
@@ -5191,7 +5191,7 @@
         <v>14195500</v>
       </c>
       <c r="H172">
-        <v>406.7586059570312</v>
+        <v>406.7585754394531</v>
       </c>
     </row>
     <row r="173">
@@ -5219,7 +5219,7 @@
         <v>19609500</v>
       </c>
       <c r="H173">
-        <v>400.0953369140625</v>
+        <v>400.0953063964844</v>
       </c>
     </row>
     <row r="174">
@@ -5359,7 +5359,7 @@
         <v>15874600</v>
       </c>
       <c r="H178">
-        <v>428.869873046875</v>
+        <v>428.8699035644531</v>
       </c>
     </row>
     <row r="179">
@@ -5387,7 +5387,7 @@
         <v>13834700</v>
       </c>
       <c r="H179">
-        <v>429.6168823242188</v>
+        <v>429.6169128417969</v>
       </c>
     </row>
     <row r="180">
@@ -5471,7 +5471,7 @@
         <v>21706600</v>
       </c>
       <c r="H182">
-        <v>436.9375305175781</v>
+        <v>436.9375610351562</v>
       </c>
     </row>
     <row r="183">
@@ -5555,7 +5555,7 @@
         <v>17015800</v>
       </c>
       <c r="H185">
-        <v>427.45556640625</v>
+        <v>427.4555969238281</v>
       </c>
     </row>
     <row r="186">
@@ -5611,7 +5611,7 @@
         <v>14492000</v>
       </c>
       <c r="H187">
-        <v>429.5870056152344</v>
+        <v>429.5870361328125</v>
       </c>
     </row>
     <row r="188">
@@ -5667,7 +5667,7 @@
         <v>16807300</v>
       </c>
       <c r="H189">
-        <v>428.5810241699219</v>
+        <v>428.5810546875</v>
       </c>
     </row>
     <row r="190">
@@ -5695,7 +5695,7 @@
         <v>19092900</v>
       </c>
       <c r="H190">
-        <v>419.0094299316406</v>
+        <v>419.0094604492188</v>
       </c>
     </row>
     <row r="191">
@@ -5723,7 +5723,7 @@
         <v>16582300</v>
       </c>
       <c r="H191">
-        <v>415.4636840820312</v>
+        <v>415.4636535644531</v>
       </c>
     </row>
     <row r="192">
@@ -5807,7 +5807,7 @@
         <v>20919800</v>
       </c>
       <c r="H194">
-        <v>407.9040222167969</v>
+        <v>407.9039916992188</v>
       </c>
     </row>
     <row r="195">
@@ -5891,7 +5891,7 @@
         <v>13848400</v>
       </c>
       <c r="H197">
-        <v>414.1788024902344</v>
+        <v>414.1788330078125</v>
       </c>
     </row>
     <row r="198">
@@ -5919,7 +5919,7 @@
         <v>14144900</v>
       </c>
       <c r="H198">
-        <v>414.6569213867188</v>
+        <v>414.6568908691406</v>
       </c>
     </row>
     <row r="199">
@@ -5947,7 +5947,7 @@
         <v>16653100</v>
       </c>
       <c r="H199">
-        <v>417.4656372070312</v>
+        <v>417.4656677246094</v>
       </c>
     </row>
     <row r="200">
@@ -6031,7 +6031,7 @@
         <v>14820000</v>
       </c>
       <c r="H202">
-        <v>415.0553283691406</v>
+        <v>415.0552978515625</v>
       </c>
     </row>
     <row r="203">
@@ -6059,7 +6059,7 @@
         <v>17145300</v>
       </c>
       <c r="H203">
-        <v>416.4895324707031</v>
+        <v>416.4895629882812</v>
       </c>
     </row>
     <row r="204">
@@ -6171,7 +6171,7 @@
         <v>13581600</v>
       </c>
       <c r="H207">
-        <v>423.0332946777344</v>
+        <v>423.0333251953125</v>
       </c>
     </row>
     <row r="208">
@@ -6227,7 +6227,7 @@
         <v>14882400</v>
       </c>
       <c r="H209">
-        <v>424.8858947753906</v>
+        <v>424.8858642578125</v>
       </c>
     </row>
     <row r="210">
@@ -6339,7 +6339,7 @@
         <v>24230400</v>
       </c>
       <c r="H213">
-        <v>408.7306518554688</v>
+        <v>408.7306823730469</v>
       </c>
     </row>
     <row r="214">
@@ -6367,7 +6367,7 @@
         <v>19672300</v>
       </c>
       <c r="H214">
-        <v>406.8282775878906</v>
+        <v>406.8283081054688</v>
       </c>
     </row>
     <row r="215">
@@ -6451,7 +6451,7 @@
         <v>19901800</v>
       </c>
       <c r="H217">
-        <v>423.7305297851562</v>
+        <v>423.7304992675781</v>
       </c>
     </row>
     <row r="218">
@@ -6563,7 +6563,7 @@
         <v>21502200</v>
       </c>
       <c r="H221">
-        <v>423.50146484375</v>
+        <v>423.5014343261719</v>
       </c>
     </row>
     <row r="222">
@@ -6675,7 +6675,7 @@
         <v>18133500</v>
       </c>
       <c r="H225">
-        <v>416.1210632324219</v>
+        <v>416.1210327148438</v>
       </c>
     </row>
     <row r="226">
@@ -9220,7 +9220,7 @@
         <v>373.1099853515625</v>
       </c>
       <c r="G316">
-        <v>30147000</v>
+        <v>30198000</v>
       </c>
       <c r="H316">
         <v>373.1099853515625</v>

</xml_diff>

<commit_message>
added note and link to repo on web-rendered page
</commit_message>
<xml_diff>
--- a/my_exported_file.xlsx
+++ b/my_exported_file.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H316"/>
+  <dimension ref="A1:H317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -627,7 +627,7 @@
         <v>27850800</v>
       </c>
       <c r="H9">
-        <v>381.0111389160156</v>
+        <v>381.0111694335938</v>
       </c>
     </row>
     <row r="10">
@@ -655,7 +655,7 @@
         <v>21645700</v>
       </c>
       <c r="H10">
-        <v>384.8150024414062</v>
+        <v>384.8150329589844</v>
       </c>
     </row>
     <row r="11">
@@ -739,7 +739,7 @@
         <v>23392100</v>
       </c>
       <c r="H13">
-        <v>390.1642150878906</v>
+        <v>390.1641845703125</v>
       </c>
     </row>
     <row r="14">
@@ -767,7 +767,7 @@
         <v>29272000</v>
       </c>
       <c r="H14">
-        <v>394.9190673828125</v>
+        <v>394.9190368652344</v>
       </c>
     </row>
     <row r="15">
@@ -795,7 +795,7 @@
         <v>27016900</v>
       </c>
       <c r="H15">
-        <v>392.7793884277344</v>
+        <v>392.7794189453125</v>
       </c>
     </row>
     <row r="16">
@@ -823,7 +823,7 @@
         <v>20525900</v>
       </c>
       <c r="H16">
-        <v>395.1468505859375</v>
+        <v>395.1468811035156</v>
       </c>
     </row>
     <row r="17">
@@ -851,7 +851,7 @@
         <v>24867000</v>
       </c>
       <c r="H17">
-        <v>398.7724304199219</v>
+        <v>398.7724914550781</v>
       </c>
     </row>
     <row r="18">
@@ -879,7 +879,7 @@
         <v>21021200</v>
       </c>
       <c r="H18">
-        <v>401.0607299804688</v>
+        <v>401.0606994628906</v>
       </c>
     </row>
     <row r="19">
@@ -907,7 +907,7 @@
         <v>17803300</v>
       </c>
       <c r="H19">
-        <v>400.1295776367188</v>
+        <v>400.1295166015625</v>
       </c>
     </row>
     <row r="20">
@@ -935,7 +935,7 @@
         <v>24510200</v>
       </c>
       <c r="H20">
-        <v>405.8650817871094</v>
+        <v>405.8650512695312</v>
       </c>
     </row>
     <row r="21">
@@ -1019,7 +1019,7 @@
         <v>30657700</v>
       </c>
       <c r="H23">
-        <v>399.9810180664062</v>
+        <v>399.98095703125</v>
       </c>
     </row>
     <row r="24">
@@ -1075,7 +1075,7 @@
         <v>25352300</v>
       </c>
       <c r="H25">
-        <v>401.8334045410156</v>
+        <v>401.8333740234375</v>
       </c>
     </row>
     <row r="26">
@@ -1103,7 +1103,7 @@
         <v>18382600</v>
       </c>
       <c r="H26">
-        <v>401.6748352050781</v>
+        <v>401.6748657226562</v>
       </c>
     </row>
     <row r="27">
@@ -1131,7 +1131,7 @@
         <v>22340500</v>
       </c>
       <c r="H27">
-        <v>410.1543273925781</v>
+        <v>410.1543579101562</v>
       </c>
     </row>
     <row r="28">
@@ -1215,7 +1215,7 @@
         <v>21202900</v>
       </c>
       <c r="H30">
-        <v>411.3529968261719</v>
+        <v>411.3529357910156</v>
       </c>
     </row>
     <row r="31">
@@ -1355,7 +1355,7 @@
         <v>24307900</v>
       </c>
       <c r="H35">
-        <v>399.7381591796875</v>
+        <v>399.7381286621094</v>
       </c>
     </row>
     <row r="36">
@@ -1383,7 +1383,7 @@
         <v>18631100</v>
       </c>
       <c r="H36">
-        <v>399.1327209472656</v>
+        <v>399.1327514648438</v>
       </c>
     </row>
     <row r="37">
@@ -1411,7 +1411,7 @@
         <v>27009900</v>
       </c>
       <c r="H37">
-        <v>408.531005859375</v>
+        <v>408.5309753417969</v>
       </c>
     </row>
     <row r="38">
@@ -1439,7 +1439,7 @@
         <v>16295900</v>
       </c>
       <c r="H38">
-        <v>407.2308959960938</v>
+        <v>407.23095703125</v>
       </c>
     </row>
     <row r="39">
@@ -1467,7 +1467,7 @@
         <v>16193500</v>
       </c>
       <c r="H39">
-        <v>404.4521484375</v>
+        <v>404.4521789550781</v>
       </c>
     </row>
     <row r="40">
@@ -1495,7 +1495,7 @@
         <v>14835800</v>
       </c>
       <c r="H40">
-        <v>404.3926391601562</v>
+        <v>404.3926086425781</v>
       </c>
     </row>
     <row r="41">
@@ -1523,7 +1523,7 @@
         <v>13183100</v>
       </c>
       <c r="H41">
-        <v>404.6307983398438</v>
+        <v>404.6307678222656</v>
       </c>
     </row>
     <row r="42">
@@ -1607,7 +1607,7 @@
         <v>17596000</v>
       </c>
       <c r="H44">
-        <v>411.7762451171875</v>
+        <v>411.7762756347656</v>
       </c>
     </row>
     <row r="45">
@@ -1635,7 +1635,7 @@
         <v>26919200</v>
       </c>
       <c r="H45">
-        <v>399.5992126464844</v>
+        <v>399.5991516113281</v>
       </c>
     </row>
     <row r="46">
@@ -1691,7 +1691,7 @@
         <v>18718500</v>
       </c>
       <c r="H47">
-        <v>406.0400390625</v>
+        <v>406.0400695800781</v>
       </c>
     </row>
     <row r="48">
@@ -1971,7 +1971,7 @@
         <v>21296200</v>
       </c>
       <c r="H57">
-        <v>426.1167602539062</v>
+        <v>426.1167297363281</v>
       </c>
     </row>
     <row r="58">
@@ -1999,7 +1999,7 @@
         <v>17636500</v>
       </c>
       <c r="H58">
-        <v>425.4915466308594</v>
+        <v>425.4915161132812</v>
       </c>
     </row>
     <row r="59">
@@ -2083,7 +2083,7 @@
         <v>16705000</v>
       </c>
       <c r="H61">
-        <v>418.2369079589844</v>
+        <v>418.2368774414062</v>
       </c>
     </row>
     <row r="62">
@@ -2251,7 +2251,7 @@
         <v>16544300</v>
       </c>
       <c r="H67">
-        <v>422.2958984375</v>
+        <v>422.2959289550781</v>
       </c>
     </row>
     <row r="68">
@@ -2307,7 +2307,7 @@
         <v>12512300</v>
       </c>
       <c r="H69">
-        <v>423.0501708984375</v>
+        <v>423.0501403808594</v>
       </c>
     </row>
     <row r="70">
@@ -2335,7 +2335,7 @@
         <v>16216600</v>
       </c>
       <c r="H70">
-        <v>420.0530395507812</v>
+        <v>420.0530700683594</v>
       </c>
     </row>
     <row r="71">
@@ -2363,7 +2363,7 @@
         <v>17966400</v>
       </c>
       <c r="H71">
-        <v>424.6876220703125</v>
+        <v>424.6876831054688</v>
       </c>
     </row>
     <row r="72">
@@ -2615,7 +2615,7 @@
         <v>15065300</v>
       </c>
       <c r="H80">
-        <v>405.9606628417969</v>
+        <v>405.9606018066406</v>
       </c>
     </row>
     <row r="81">
@@ -2643,7 +2643,7 @@
         <v>40586500</v>
       </c>
       <c r="H81">
-        <v>396.0165710449219</v>
+        <v>396.0165405273438</v>
       </c>
     </row>
     <row r="82">
@@ -2699,7 +2699,7 @@
         <v>19582100</v>
       </c>
       <c r="H83">
-        <v>399.2022399902344</v>
+        <v>399.2022094726562</v>
       </c>
     </row>
     <row r="84">
@@ -2727,7 +2727,7 @@
         <v>28781400</v>
       </c>
       <c r="H84">
-        <v>386.380126953125</v>
+        <v>386.3800964355469</v>
       </c>
     </row>
     <row r="85">
@@ -2755,7 +2755,7 @@
         <v>23562500</v>
       </c>
       <c r="H85">
-        <v>391.9476318359375</v>
+        <v>391.9476013183594</v>
       </c>
     </row>
     <row r="86">
@@ -2783,7 +2783,7 @@
         <v>17709400</v>
       </c>
       <c r="H86">
-        <v>394.8255920410156</v>
+        <v>394.8256530761719</v>
       </c>
     </row>
     <row r="87">
@@ -2867,7 +2867,7 @@
         <v>20018200</v>
       </c>
       <c r="H89">
-        <v>406.2384948730469</v>
+        <v>406.238525390625</v>
       </c>
     </row>
     <row r="90">
@@ -2923,7 +2923,7 @@
         <v>14689700</v>
       </c>
       <c r="H91">
-        <v>409.1959533691406</v>
+        <v>409.1959228515625</v>
       </c>
     </row>
     <row r="92">
@@ -3035,7 +3035,7 @@
         <v>22239500</v>
       </c>
       <c r="H95">
-        <v>420.6317138671875</v>
+        <v>420.6317443847656</v>
       </c>
     </row>
     <row r="96">
@@ -3147,7 +3147,7 @@
         <v>21453300</v>
       </c>
       <c r="H99">
-        <v>426.5572814941406</v>
+        <v>426.5572509765625</v>
       </c>
     </row>
     <row r="100">
@@ -3175,7 +3175,7 @@
         <v>18073700</v>
       </c>
       <c r="H100">
-        <v>428.0286865234375</v>
+        <v>428.0287170410156</v>
       </c>
     </row>
     <row r="101">
@@ -3259,7 +3259,7 @@
         <v>15718000</v>
       </c>
       <c r="H103">
-        <v>427.829833984375</v>
+        <v>427.8298645019531</v>
       </c>
     </row>
     <row r="104">
@@ -3707,7 +3707,7 @@
         <v>19877400</v>
       </c>
       <c r="H119">
-        <v>443.120849609375</v>
+        <v>443.1208801269531</v>
       </c>
     </row>
     <row r="120">
@@ -3763,7 +3763,7 @@
         <v>15913700</v>
       </c>
       <c r="H121">
-        <v>445.0794982910156</v>
+        <v>445.0794677734375</v>
       </c>
     </row>
     <row r="122">
@@ -3875,7 +3875,7 @@
         <v>28362300</v>
       </c>
       <c r="H125">
-        <v>444.3636474609375</v>
+        <v>444.3636169433594</v>
       </c>
     </row>
     <row r="126">
@@ -3903,7 +3903,7 @@
         <v>17662800</v>
       </c>
       <c r="H126">
-        <v>454.0870361328125</v>
+        <v>454.0870056152344</v>
       </c>
     </row>
     <row r="127">
@@ -4099,7 +4099,7 @@
         <v>23111200</v>
       </c>
       <c r="H133">
-        <v>452.0687561035156</v>
+        <v>452.0687866210938</v>
       </c>
     </row>
     <row r="134">
@@ -4155,7 +4155,7 @@
         <v>14429400</v>
       </c>
       <c r="H135">
-        <v>451.3330688476562</v>
+        <v>451.3330383300781</v>
       </c>
     </row>
     <row r="136">
@@ -4435,7 +4435,7 @@
         <v>15125800</v>
       </c>
       <c r="H145">
-        <v>424.2606201171875</v>
+        <v>424.2606506347656</v>
       </c>
     </row>
     <row r="146">
@@ -4491,7 +4491,7 @@
         <v>42891400</v>
       </c>
       <c r="H147">
-        <v>415.9291381835938</v>
+        <v>415.9291076660156</v>
       </c>
     </row>
     <row r="148">
@@ -4519,7 +4519,7 @@
         <v>30296400</v>
       </c>
       <c r="H148">
-        <v>414.6962890625</v>
+        <v>414.6962585449219</v>
       </c>
     </row>
     <row r="149">
@@ -4575,7 +4575,7 @@
         <v>40709200</v>
       </c>
       <c r="H150">
-        <v>392.8633422851562</v>
+        <v>392.8633728027344</v>
       </c>
     </row>
     <row r="151">
@@ -4659,7 +4659,7 @@
         <v>20203000</v>
       </c>
       <c r="H153">
-        <v>400.3597412109375</v>
+        <v>400.3597106933594</v>
       </c>
     </row>
     <row r="154">
@@ -4855,7 +4855,7 @@
         <v>15234000</v>
       </c>
       <c r="H160">
-        <v>419.8460998535156</v>
+        <v>419.8460693359375</v>
       </c>
     </row>
     <row r="161">
@@ -4939,7 +4939,7 @@
         <v>19361900</v>
       </c>
       <c r="H163">
-        <v>413.8899841308594</v>
+        <v>413.8899536132812</v>
       </c>
     </row>
     <row r="164">
@@ -4995,7 +4995,7 @@
         <v>13152800</v>
       </c>
       <c r="H165">
-        <v>411.8381958007812</v>
+        <v>411.8382263183594</v>
       </c>
     </row>
     <row r="166">
@@ -5023,7 +5023,7 @@
         <v>13492900</v>
       </c>
       <c r="H166">
-        <v>412.1867980957031</v>
+        <v>412.1868286132812</v>
       </c>
     </row>
     <row r="167">
@@ -5051,7 +5051,7 @@
         <v>14882700</v>
       </c>
       <c r="H167">
-        <v>408.9597778320312</v>
+        <v>408.9597473144531</v>
       </c>
     </row>
     <row r="168">
@@ -5191,7 +5191,7 @@
         <v>14195500</v>
       </c>
       <c r="H172">
-        <v>406.7585754394531</v>
+        <v>406.7586059570312</v>
       </c>
     </row>
     <row r="173">
@@ -5219,7 +5219,7 @@
         <v>19609500</v>
       </c>
       <c r="H173">
-        <v>400.0953063964844</v>
+        <v>400.0953369140625</v>
       </c>
     </row>
     <row r="174">
@@ -5359,7 +5359,7 @@
         <v>15874600</v>
       </c>
       <c r="H178">
-        <v>428.8699035644531</v>
+        <v>428.869873046875</v>
       </c>
     </row>
     <row r="179">
@@ -5387,7 +5387,7 @@
         <v>13834700</v>
       </c>
       <c r="H179">
-        <v>429.6169128417969</v>
+        <v>429.6168823242188</v>
       </c>
     </row>
     <row r="180">
@@ -5471,7 +5471,7 @@
         <v>21706600</v>
       </c>
       <c r="H182">
-        <v>436.9375610351562</v>
+        <v>436.9375305175781</v>
       </c>
     </row>
     <row r="183">
@@ -5555,7 +5555,7 @@
         <v>17015800</v>
       </c>
       <c r="H185">
-        <v>427.4555969238281</v>
+        <v>427.45556640625</v>
       </c>
     </row>
     <row r="186">
@@ -5611,7 +5611,7 @@
         <v>14492000</v>
       </c>
       <c r="H187">
-        <v>429.5870361328125</v>
+        <v>429.5870056152344</v>
       </c>
     </row>
     <row r="188">
@@ -5667,7 +5667,7 @@
         <v>16807300</v>
       </c>
       <c r="H189">
-        <v>428.5810546875</v>
+        <v>428.5810241699219</v>
       </c>
     </row>
     <row r="190">
@@ -5695,7 +5695,7 @@
         <v>19092900</v>
       </c>
       <c r="H190">
-        <v>419.0094604492188</v>
+        <v>419.0094299316406</v>
       </c>
     </row>
     <row r="191">
@@ -5723,7 +5723,7 @@
         <v>16582300</v>
       </c>
       <c r="H191">
-        <v>415.4636535644531</v>
+        <v>415.4636840820312</v>
       </c>
     </row>
     <row r="192">
@@ -5807,7 +5807,7 @@
         <v>20919800</v>
       </c>
       <c r="H194">
-        <v>407.9039916992188</v>
+        <v>407.9040222167969</v>
       </c>
     </row>
     <row r="195">
@@ -5891,7 +5891,7 @@
         <v>13848400</v>
       </c>
       <c r="H197">
-        <v>414.1788330078125</v>
+        <v>414.1788024902344</v>
       </c>
     </row>
     <row r="198">
@@ -5919,7 +5919,7 @@
         <v>14144900</v>
       </c>
       <c r="H198">
-        <v>414.6568908691406</v>
+        <v>414.6569213867188</v>
       </c>
     </row>
     <row r="199">
@@ -5947,7 +5947,7 @@
         <v>16653100</v>
       </c>
       <c r="H199">
-        <v>417.4656677246094</v>
+        <v>417.4656372070312</v>
       </c>
     </row>
     <row r="200">
@@ -6031,7 +6031,7 @@
         <v>14820000</v>
       </c>
       <c r="H202">
-        <v>415.0552978515625</v>
+        <v>415.0553283691406</v>
       </c>
     </row>
     <row r="203">
@@ -6059,7 +6059,7 @@
         <v>17145300</v>
       </c>
       <c r="H203">
-        <v>416.4895629882812</v>
+        <v>416.4895324707031</v>
       </c>
     </row>
     <row r="204">
@@ -6171,7 +6171,7 @@
         <v>13581600</v>
       </c>
       <c r="H207">
-        <v>423.0333251953125</v>
+        <v>423.0332946777344</v>
       </c>
     </row>
     <row r="208">
@@ -6227,7 +6227,7 @@
         <v>14882400</v>
       </c>
       <c r="H209">
-        <v>424.8858642578125</v>
+        <v>424.8858947753906</v>
       </c>
     </row>
     <row r="210">
@@ -6339,7 +6339,7 @@
         <v>24230400</v>
       </c>
       <c r="H213">
-        <v>408.7306823730469</v>
+        <v>408.7306518554688</v>
       </c>
     </row>
     <row r="214">
@@ -6367,7 +6367,7 @@
         <v>19672300</v>
       </c>
       <c r="H214">
-        <v>406.8283081054688</v>
+        <v>406.8282775878906</v>
       </c>
     </row>
     <row r="215">
@@ -6451,7 +6451,7 @@
         <v>19901800</v>
       </c>
       <c r="H217">
-        <v>423.7304992675781</v>
+        <v>423.7305297851562</v>
       </c>
     </row>
     <row r="218">
@@ -6563,7 +6563,7 @@
         <v>21502200</v>
       </c>
       <c r="H221">
-        <v>423.5014343261719</v>
+        <v>423.50146484375</v>
       </c>
     </row>
     <row r="222">
@@ -6675,7 +6675,7 @@
         <v>18133500</v>
       </c>
       <c r="H225">
-        <v>416.1210327148438</v>
+        <v>416.1210632324219</v>
       </c>
     </row>
     <row r="226">
@@ -9224,6 +9224,34 @@
       </c>
       <c r="H316">
         <v>373.1099853515625</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B317" s="2">
+        <v>45751</v>
+      </c>
+      <c r="C317">
+        <v>364.1300048828125</v>
+      </c>
+      <c r="D317">
+        <v>374.5899963378906</v>
+      </c>
+      <c r="E317">
+        <v>359.4800109863281</v>
+      </c>
+      <c r="F317">
+        <v>359.8399963378906</v>
+      </c>
+      <c r="G317">
+        <v>49138700</v>
+      </c>
+      <c r="H317">
+        <v>359.8399963378906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>